<commit_message>
confirm libre json2xls convert array
</commit_message>
<xml_diff>
--- a/generate_excel/data.xlsx
+++ b/generate_excel/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7" count="7">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10" count="10">
   <x:si>
     <x:t>foo</x:t>
   </x:si>
@@ -34,7 +34,16 @@
     <x:t>moo</x:t>
   </x:si>
   <x:si>
-    <x:t>Mon Jun 14 2021</x:t>
+    <x:t>Fri Jun 18 2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>bar 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>moo 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Wed May 19 2021</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -425,6 +434,20 @@
         <x:v>6</x:v>
       </x:c>
     </x:row>
+    <x:row r="3" spans="1:4">
+      <x:c r="A3" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="n">
+        <x:v>1234</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>